<commit_message>
update analysis for submission
</commit_message>
<xml_diff>
--- a/results/dins30_cameraPR/dins30_cameraPR.xlsx
+++ b/results/dins30_cameraPR/dins30_cameraPR.xlsx
@@ -360,7 +360,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -374,17 +374,17 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>EMY.z.Direction</t>
+          <t>EMY.chisq.Direction</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>EMY.z.p</t>
+          <t>EMY.chisq.p</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>EMY.z.FDR</t>
+          <t>EMY.chisq.FDR</t>
         </is>
       </c>
     </row>
@@ -400,69 +400,69 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>0.000181</v>
+        <v>3.74e-007</v>
       </c>
       <c r="E2">
-        <v>0.013</v>
+        <v>2.66e-005</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2">
-        <f>HYPERLINK("pathways/Inositol_Metabolism.csv","Inositol Metabolism")</f>
+        <f>HYPERLINK("pathways/Sphingolipid_Metabolism.csv","Sphingolipid Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0.0508</v>
+        <v>0.0509</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2">
-        <f>HYPERLINK("pathways/Phosphatidylinositol_Phosphate_Metabolism.csv","Phosphatidylinositol Phosphate Metabolism")</f>
+        <f>HYPERLINK("pathways/Phospholipid_Biosynthesis.csv","Phospholipid Biosynthesis")</f>
         <v>0</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4">
-        <v>0.0901</v>
+        <v>0.08989999999999999</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2">
-        <f>HYPERLINK("pathways/Sphingolipid_Metabolism.csv","Sphingolipid Metabolism")</f>
+        <f>HYPERLINK("pathways/Fatty_acid_Metabolism.csv","Fatty acid Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5">
-        <v>0.136</v>
+        <v>0.117</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2">
-        <f>HYPERLINK("pathways/Fatty_acid_Metabolism.csv","Fatty acid Metabolism")</f>
+        <f>HYPERLINK("pathways/Mitochondrial_Beta_Oxidation_of_Short_Chain_Saturated_Fatty_Acids.csv","Mitochondrial Beta-Oxidation of Short Chain Saturated Fatty Acids")</f>
         <v>0</v>
       </c>
       <c r="B6">
@@ -472,15 +472,15 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>0.147</v>
+        <v>0.127</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2">
-        <f>HYPERLINK("pathways/Phospholipid_Biosynthesis.csv","Phospholipid Biosynthesis")</f>
+        <f>HYPERLINK("pathways/Taurine_and_Hypotaurine_Metabolism.csv","Taurine and Hypotaurine Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B7">
@@ -490,195 +490,195 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>0.158</v>
+        <v>0.168</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2">
-        <f>HYPERLINK("pathways/Mitochondrial_Beta_Oxidation_of_Short_Chain_Saturated_Fatty_Acids.csv","Mitochondrial Beta-Oxidation of Short Chain Saturated Fatty Acids")</f>
+        <f>HYPERLINK("pathways/Amino_Sugar_Metabolism.csv","Amino Sugar Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8">
-        <v>0.171</v>
+        <v>0.182</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2">
-        <f>HYPERLINK("pathways/Phenylacetate_Metabolism.csv","Phenylacetate Metabolism")</f>
+        <f>HYPERLINK("pathways/Pentose_Phosphate_Pathway.csv","Pentose Phosphate Pathway")</f>
         <v>0</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9">
-        <v>0.179</v>
+        <v>0.229</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2">
-        <f>HYPERLINK("pathways/Taurine_and_Hypotaurine_Metabolism.csv","Taurine and Hypotaurine Metabolism")</f>
+        <f>HYPERLINK("pathways/Retinol_Metabolism.csv","Retinol Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10">
-        <v>0.209</v>
+        <v>0.323</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2">
-        <f>HYPERLINK("pathways/Pentose_Phosphate_Pathway.csv","Pentose Phosphate Pathway")</f>
+        <f>HYPERLINK("pathways/Nicotinate_and_Nicotinamide_Metabolism.csv","Nicotinate and Nicotinamide Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11">
-        <v>0.223</v>
+        <v>0.34</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2">
-        <f>HYPERLINK("pathways/Nicotinate_and_Nicotinamide_Metabolism.csv","Nicotinate and Nicotinamide Metabolism")</f>
+        <f>HYPERLINK("pathways/Phosphatidylinositol_Phosphate_Metabolism.csv","Phosphatidylinositol Phosphate Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B12">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12">
-        <v>0.3</v>
+        <v>0.342</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2">
-        <f>HYPERLINK("pathways/Amino_Sugar_Metabolism.csv","Amino Sugar Metabolism")</f>
+        <f>HYPERLINK("pathways/Phenylacetate_Metabolism.csv","Phenylacetate Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B13">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13">
-        <v>0.395</v>
+        <v>0.422</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2">
-        <f>HYPERLINK("pathways/Ammonia_Recycling.csv","Ammonia Recycling")</f>
+        <f>HYPERLINK("pathways/Phenylalanine_and_Tyrosine_Metabolism.csv","Phenylalanine and Tyrosine Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B14">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14">
-        <v>0.48</v>
+        <v>0.457</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2">
-        <f>HYPERLINK("pathways/Lactose_Synthesis.csv","Lactose Synthesis")</f>
+        <f>HYPERLINK("pathways/Galactose_Metabolism.csv","Galactose Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15">
-        <v>0.495</v>
+        <v>0.462</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2">
-        <f>HYPERLINK("pathways/Phenylalanine_and_Tyrosine_Metabolism.csv","Phenylalanine and Tyrosine Metabolism")</f>
+        <f>HYPERLINK("pathways/Cysteine_Metabolism.csv","Cysteine Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B16">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C16">
         <v>-1</v>
       </c>
       <c r="D16">
-        <v>0.502</v>
+        <v>0.501</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2">
-        <f>HYPERLINK("pathways/Retinol_Metabolism.csv","Retinol Metabolism")</f>
+        <f>HYPERLINK("pathways/Methylhistidine_Metabolism.csv","Methylhistidine Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B17">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C17">
         <v>-1</v>
       </c>
       <c r="D17">
-        <v>0.514</v>
+        <v>0.52</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2">
-        <f>HYPERLINK("pathways/Methylhistidine_Metabolism.csv","Methylhistidine Metabolism")</f>
+        <f>HYPERLINK("pathways/Lactose_Synthesis.csv","Lactose Synthesis")</f>
         <v>0</v>
       </c>
       <c r="B18">
@@ -688,267 +688,267 @@
         <v>-1</v>
       </c>
       <c r="D18">
-        <v>0.581</v>
+        <v>0.529</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2">
-        <f>HYPERLINK("pathways/Aspartate_Metabolism.csv","Aspartate Metabolism")</f>
+        <f>HYPERLINK("pathways/Beta_Alanine_Metabolism.csv","Beta-Alanine Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B19">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C19">
         <v>-1</v>
       </c>
       <c r="D19">
-        <v>0.593</v>
+        <v>0.542</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2">
-        <f>HYPERLINK("pathways/Sulfate_Sulfite_Metabolism.csv","Sulfate/Sulfite Metabolism")</f>
+        <f>HYPERLINK("pathways/Glycerol_Phosphate_Shuttle.csv","Glycerol Phosphate Shuttle")</f>
         <v>0</v>
       </c>
       <c r="B20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C20">
         <v>-1</v>
       </c>
       <c r="D20">
-        <v>0.613</v>
+        <v>0.542</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2">
-        <f>HYPERLINK("pathways/Histidine_Metabolism.csv","Histidine Metabolism")</f>
+        <f>HYPERLINK("pathways/Fructose_and_Mannose_Degradation.csv","Fructose and Mannose Degradation")</f>
         <v>0</v>
       </c>
       <c r="B21">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C21">
         <v>-1</v>
       </c>
       <c r="D21">
-        <v>0.658</v>
+        <v>0.546</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2">
-        <f>HYPERLINK("pathways/Cysteine_Metabolism.csv","Cysteine Metabolism")</f>
+        <f>HYPERLINK("pathways/Histidine_Metabolism.csv","Histidine Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B22">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C22">
         <v>-1</v>
       </c>
       <c r="D22">
-        <v>0.67</v>
+        <v>0.5620000000000001</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2">
-        <f>HYPERLINK("pathways/Beta_Alanine_Metabolism.csv","Beta-Alanine Metabolism")</f>
+        <f>HYPERLINK("pathways/Sulfate_Sulfite_Metabolism.csv","Sulfate/Sulfite Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B23">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C23">
         <v>-1</v>
       </c>
       <c r="D23">
-        <v>0.6770000000000001</v>
+        <v>0.574</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2">
-        <f>HYPERLINK("pathways/Propanoate_Metabolism.csv","Propanoate Metabolism")</f>
+        <f>HYPERLINK("pathways/Warburg_Effect.csv","Warburg Effect")</f>
         <v>0</v>
       </c>
       <c r="B24">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C24">
         <v>-1</v>
       </c>
       <c r="D24">
-        <v>0.6780000000000001</v>
+        <v>0.641</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2">
-        <f>HYPERLINK("pathways/Glycerol_Phosphate_Shuttle.csv","Glycerol Phosphate Shuttle")</f>
+        <f>HYPERLINK("pathways/Pyrimidine_Metabolism.csv","Pyrimidine Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B25">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C25">
         <v>-1</v>
       </c>
       <c r="D25">
-        <v>0.7</v>
+        <v>0.646</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2">
-        <f>HYPERLINK("pathways/Pantothenate_and_CoA_Biosynthesis.csv","Pantothenate and CoA Biosynthesis")</f>
+        <f>HYPERLINK("pathways/Bile_Acid_Biosynthesis.csv","Bile Acid Biosynthesis")</f>
         <v>0</v>
       </c>
       <c r="B26">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C26">
         <v>-1</v>
       </c>
       <c r="D26">
-        <v>0.708</v>
+        <v>0.648</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2">
-        <f>HYPERLINK("pathways/Malate_Aspartate_Shuttle.csv","Malate-Aspartate Shuttle")</f>
+        <f>HYPERLINK("pathways/Selenoamino_Acid_Metabolism.csv","Selenoamino Acid Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B27">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C27">
         <v>-1</v>
       </c>
       <c r="D27">
-        <v>0.711</v>
+        <v>0.655</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2">
-        <f>HYPERLINK("pathways/Riboflavin_Metabolism.csv","Riboflavin Metabolism")</f>
+        <f>HYPERLINK("pathways/Butyrate_Metabolism.csv","Butyrate Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C28">
         <v>-1</v>
       </c>
       <c r="D28">
-        <v>0.731</v>
+        <v>0.701</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2">
-        <f>HYPERLINK("pathways/Fructose_and_Mannose_Degradation.csv","Fructose and Mannose Degradation")</f>
+        <f>HYPERLINK("pathways/Ethanol_Degradation.csv","Ethanol Degradation")</f>
         <v>0</v>
       </c>
       <c r="B29">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C29">
         <v>-1</v>
       </c>
       <c r="D29">
-        <v>0.734</v>
+        <v>0.701</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2">
-        <f>HYPERLINK("pathways/Arachidonic_Acid_Metabolism.csv","Arachidonic Acid Metabolism")</f>
+        <f>HYPERLINK("pathways/Pantothenate_and_CoA_Biosynthesis.csv","Pantothenate and CoA Biosynthesis")</f>
         <v>0</v>
       </c>
       <c r="B30">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C30">
         <v>-1</v>
       </c>
       <c r="D30">
-        <v>0.735</v>
+        <v>0.701</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2">
-        <f>HYPERLINK("pathways/Spermidine_and_Spermine_Biosynthesis.csv","Spermidine and Spermine Biosynthesis")</f>
+        <f>HYPERLINK("pathways/Tryptophan_Metabolism.csv","Tryptophan Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B31">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C31">
         <v>-1</v>
       </c>
       <c r="D31">
-        <v>0.749</v>
+        <v>0.712</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2">
-        <f>HYPERLINK("pathways/Purine_Metabolism.csv","Purine Metabolism")</f>
+        <f>HYPERLINK("pathways/Glycolysis.csv","Glycolysis")</f>
         <v>0</v>
       </c>
       <c r="B32">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C32">
         <v>-1</v>
       </c>
       <c r="D32">
-        <v>0.75</v>
+        <v>0.715</v>
       </c>
       <c r="E32">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2">
-        <f>HYPERLINK("pathways/Homocysteine_Degradation.csv","Homocysteine Degradation")</f>
+        <f>HYPERLINK("pathways/Androgen_and_Estrogen_Metabolism.csv","Androgen and Estrogen Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B33">
@@ -958,69 +958,69 @@
         <v>-1</v>
       </c>
       <c r="D33">
-        <v>0.762</v>
+        <v>0.718</v>
       </c>
       <c r="E33">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2">
-        <f>HYPERLINK("pathways/Bile_Acid_Biosynthesis.csv","Bile Acid Biosynthesis")</f>
+        <f>HYPERLINK("pathways/Arachidonic_Acid_Metabolism.csv","Arachidonic Acid Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B34">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C34">
         <v>-1</v>
       </c>
       <c r="D34">
-        <v>0.773</v>
+        <v>0.733</v>
       </c>
       <c r="E34">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2">
-        <f>HYPERLINK("pathways/Methionine_Metabolism.csv","Methionine Metabolism")</f>
+        <f>HYPERLINK("pathways/Ammonia_Recycling.csv","Ammonia Recycling")</f>
         <v>0</v>
       </c>
       <c r="B35">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C35">
         <v>-1</v>
       </c>
       <c r="D35">
-        <v>0.781</v>
+        <v>0.738</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2">
-        <f>HYPERLINK("pathways/Betaine_Metabolism.csv","Betaine Metabolism")</f>
+        <f>HYPERLINK("pathways/Aspartate_Metabolism.csv","Aspartate Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B36">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C36">
         <v>-1</v>
       </c>
       <c r="D36">
-        <v>0.794</v>
+        <v>0.739</v>
       </c>
       <c r="E36">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2">
-        <f>HYPERLINK("pathways/Galactose_Metabolism.csv","Galactose Metabolism")</f>
+        <f>HYPERLINK("pathways/Propanoate_Metabolism.csv","Propanoate Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B37">
@@ -1030,69 +1030,69 @@
         <v>-1</v>
       </c>
       <c r="D37">
-        <v>0.8020000000000001</v>
+        <v>0.743</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2">
-        <f>HYPERLINK("pathways/Selenoamino_Acid_Metabolism.csv","Selenoamino Acid Metabolism")</f>
+        <f>HYPERLINK("pathways/Malate_Aspartate_Shuttle.csv","Malate-Aspartate Shuttle")</f>
         <v>0</v>
       </c>
       <c r="B38">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C38">
         <v>-1</v>
       </c>
       <c r="D38">
-        <v>0.841</v>
+        <v>0.782</v>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2">
-        <f>HYPERLINK("pathways/Pyrimidine_Metabolism.csv","Pyrimidine Metabolism")</f>
+        <f>HYPERLINK("pathways/Riboflavin_Metabolism.csv","Riboflavin Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B39">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C39">
         <v>-1</v>
       </c>
       <c r="D39">
-        <v>0.842</v>
+        <v>0.8010000000000001</v>
       </c>
       <c r="E39">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2">
-        <f>HYPERLINK("pathways/Steroid_Biosynthesis.csv","Steroid Biosynthesis")</f>
+        <f>HYPERLINK("pathways/Homocysteine_Degradation.csv","Homocysteine Degradation")</f>
         <v>0</v>
       </c>
       <c r="B40">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C40">
         <v>-1</v>
       </c>
       <c r="D40">
-        <v>0.868</v>
+        <v>0.8090000000000001</v>
       </c>
       <c r="E40">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2">
-        <f>HYPERLINK("pathways/Glutathione_Metabolism.csv","Glutathione Metabolism")</f>
+        <f>HYPERLINK("pathways/Spermidine_and_Spermine_Biosynthesis.csv","Spermidine and Spermine Biosynthesis")</f>
         <v>0</v>
       </c>
       <c r="B41">
@@ -1102,478 +1102,478 @@
         <v>-1</v>
       </c>
       <c r="D41">
-        <v>0.87</v>
+        <v>0.832</v>
       </c>
       <c r="E41">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2">
-        <f>HYPERLINK("pathways/Glycolysis.csv","Glycolysis")</f>
+        <f>HYPERLINK("pathways/Steroid_Biosynthesis.csv","Steroid Biosynthesis")</f>
         <v>0</v>
       </c>
       <c r="B42">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C42">
         <v>-1</v>
       </c>
       <c r="D42">
-        <v>0.873</v>
+        <v>0.835</v>
       </c>
       <c r="E42">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2">
-        <f>HYPERLINK("pathways/Butyrate_Metabolism.csv","Butyrate Metabolism")</f>
+        <f>HYPERLINK("pathways/Gluconeogenesis.csv","Gluconeogenesis")</f>
         <v>0</v>
       </c>
       <c r="B43">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C43">
         <v>-1</v>
       </c>
       <c r="D43">
-        <v>0.906</v>
+        <v>0.836</v>
       </c>
       <c r="E43">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2">
-        <f>HYPERLINK("pathways/Ethanol_Degradation.csv","Ethanol Degradation")</f>
+        <f>HYPERLINK("pathways/Betaine_Metabolism.csv","Betaine Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B44">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C44">
         <v>-1</v>
       </c>
       <c r="D44">
-        <v>0.914</v>
+        <v>0.842</v>
       </c>
       <c r="E44">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2">
-        <f>HYPERLINK("pathways/Starch_and_Sucrose_Metabolism.csv","Starch and Sucrose Metabolism")</f>
+        <f>HYPERLINK("pathways/Vitamin_B6_Metabolism.csv","Vitamin B6 Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B45">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C45">
         <v>-1</v>
       </c>
       <c r="D45">
-        <v>0.92</v>
+        <v>0.847</v>
       </c>
       <c r="E45">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2">
-        <f>HYPERLINK("pathways/Porphyrin_Metabolism.csv","Porphyrin Metabolism")</f>
+        <f>HYPERLINK("pathways/Glucose_Alanine_Cycle.csv","Glucose-Alanine Cycle")</f>
         <v>0</v>
       </c>
       <c r="B46">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C46">
         <v>-1</v>
       </c>
       <c r="D46">
-        <v>0.9340000000000001</v>
+        <v>0.85</v>
       </c>
       <c r="E46">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2">
-        <f>HYPERLINK("pathways/Androgen_and_Estrogen_Metabolism.csv","Androgen and Estrogen Metabolism")</f>
+        <f>HYPERLINK("pathways/Purine_Metabolism.csv","Purine Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B47">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C47">
         <v>-1</v>
       </c>
       <c r="D47">
-        <v>0.9360000000000001</v>
+        <v>0.852</v>
       </c>
       <c r="E47">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2">
-        <f>HYPERLINK("pathways/Urea_Cycle.csv","Urea Cycle")</f>
+        <f>HYPERLINK("pathways/Glycerolipid_Metabolism.csv","Glycerolipid Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B48">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C48">
         <v>-1</v>
       </c>
       <c r="D48">
-        <v>0.9370000000000001</v>
+        <v>0.854</v>
       </c>
       <c r="E48">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2">
-        <f>HYPERLINK("pathways/Warburg_Effect.csv","Warburg Effect")</f>
+        <f>HYPERLINK("pathways/Glutathione_Metabolism.csv","Glutathione Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B49">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C49">
         <v>-1</v>
       </c>
       <c r="D49">
-        <v>0.94</v>
+        <v>0.856</v>
       </c>
       <c r="E49">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2">
-        <f>HYPERLINK("pathways/Lysine_Degradation.csv","Lysine Degradation")</f>
+        <f>HYPERLINK("pathways/Urea_Cycle.csv","Urea Cycle")</f>
         <v>0</v>
       </c>
       <c r="B50">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C50">
         <v>-1</v>
       </c>
       <c r="D50">
-        <v>0.944</v>
+        <v>0.866</v>
       </c>
       <c r="E50">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2">
-        <f>HYPERLINK("pathways/Vitamin_B6_Metabolism.csv","Vitamin B6 Metabolism")</f>
+        <f>HYPERLINK("pathways/Starch_and_Sucrose_Metabolism.csv","Starch and Sucrose Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B51">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C51">
         <v>-1</v>
       </c>
       <c r="D51">
-        <v>0.952</v>
+        <v>0.867</v>
       </c>
       <c r="E51">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2">
-        <f>HYPERLINK("pathways/Glycerolipid_Metabolism.csv","Glycerolipid Metabolism")</f>
+        <f>HYPERLINK("pathways/Porphyrin_Metabolism.csv","Porphyrin Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B52">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C52">
         <v>-1</v>
       </c>
       <c r="D52">
-        <v>0.957</v>
+        <v>0.889</v>
       </c>
       <c r="E52">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2">
-        <f>HYPERLINK("pathways/Thyroid_hormone_synthesis.csv","Thyroid hormone synthesis")</f>
+        <f>HYPERLINK("pathways/Mitochondrial_Electron_Transport_Chain.csv","Mitochondrial Electron Transport Chain")</f>
         <v>0</v>
       </c>
       <c r="B53">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C53">
         <v>-1</v>
       </c>
       <c r="D53">
-        <v>0.957</v>
+        <v>0.889</v>
       </c>
       <c r="E53">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2">
-        <f>HYPERLINK("pathways/Degradation_of_Superoxides.csv","Degradation of Superoxides")</f>
+        <f>HYPERLINK("pathways/Tyrosine_Metabolism.csv","Tyrosine Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B54">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C54">
         <v>-1</v>
       </c>
       <c r="D54">
-        <v>0.965</v>
+        <v>0.9</v>
       </c>
       <c r="E54">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2">
-        <f>HYPERLINK("pathways/Mitochondrial_Electron_Transport_Chain.csv","Mitochondrial Electron Transport Chain")</f>
+        <f>HYPERLINK("pathways/Thyroid_hormone_synthesis.csv","Thyroid hormone synthesis")</f>
         <v>0</v>
       </c>
       <c r="B55">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C55">
         <v>-1</v>
       </c>
       <c r="D55">
-        <v>0.969</v>
+        <v>0.901</v>
       </c>
       <c r="E55">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2">
-        <f>HYPERLINK("pathways/Tyrosine_Metabolism.csv","Tyrosine Metabolism")</f>
+        <f>HYPERLINK("pathways/Alanine_Metabolism.csv","Alanine Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B56">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C56">
         <v>-1</v>
       </c>
       <c r="D56">
-        <v>0.974</v>
+        <v>0.902</v>
       </c>
       <c r="E56">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2">
-        <f>HYPERLINK("pathways/Alanine_Metabolism.csv","Alanine Metabolism")</f>
+        <f>HYPERLINK("pathways/Lysine_Degradation.csv","Lysine Degradation")</f>
         <v>0</v>
       </c>
       <c r="B57">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C57">
         <v>-1</v>
       </c>
       <c r="D57">
-        <v>0.977</v>
+        <v>0.902</v>
       </c>
       <c r="E57">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2">
-        <f>HYPERLINK("pathways/Arginine_and_Proline_Metabolism.csv","Arginine and Proline Metabolism")</f>
+        <f>HYPERLINK("pathways/Glutamate_Metabolism.csv","Glutamate Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B58">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C58">
         <v>-1</v>
       </c>
       <c r="D58">
-        <v>0.978</v>
+        <v>0.902</v>
       </c>
       <c r="E58">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2">
-        <f>HYPERLINK("pathways/Steroidogenesis.csv","Steroidogenesis")</f>
+        <f>HYPERLINK("pathways/Pyruvate_Metabolism.csv","Pyruvate Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B59">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C59">
         <v>-1</v>
       </c>
       <c r="D59">
-        <v>0.978</v>
+        <v>0.905</v>
       </c>
       <c r="E59">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2">
-        <f>HYPERLINK("pathways/Tryptophan_Metabolism.csv","Tryptophan Metabolism")</f>
+        <f>HYPERLINK("pathways/Transfer_of_Acetyl_Groups_into_Mitochondria.csv","Transfer of Acetyl Groups into Mitochondria")</f>
         <v>0</v>
       </c>
       <c r="B60">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C60">
         <v>-1</v>
       </c>
       <c r="D60">
-        <v>0.979</v>
+        <v>0.91</v>
       </c>
       <c r="E60">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="2">
-        <f>HYPERLINK("pathways/Glutamate_Metabolism.csv","Glutamate Metabolism")</f>
+        <f>HYPERLINK("pathways/Catecholamine_Biosynthesis.csv","Catecholamine Biosynthesis")</f>
         <v>0</v>
       </c>
       <c r="B61">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C61">
         <v>-1</v>
       </c>
       <c r="D61">
-        <v>0.979</v>
+        <v>0.915</v>
       </c>
       <c r="E61">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="2">
-        <f>HYPERLINK("pathways/Carnitine_Synthesis.csv","Carnitine Synthesis")</f>
+        <f>HYPERLINK("pathways/Oxidation_of_Branched_Chain_Fatty_Acids.csv","Oxidation of Branched Chain Fatty Acids")</f>
         <v>0</v>
       </c>
       <c r="B62">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C62">
         <v>-1</v>
       </c>
       <c r="D62">
-        <v>0.982</v>
+        <v>0.915</v>
       </c>
       <c r="E62">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="2">
-        <f>HYPERLINK("pathways/Gluconeogenesis.csv","Gluconeogenesis")</f>
+        <f>HYPERLINK("pathways/Steroidogenesis.csv","Steroidogenesis")</f>
         <v>0</v>
       </c>
       <c r="B63">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C63">
         <v>-1</v>
       </c>
       <c r="D63">
-        <v>0.986</v>
+        <v>0.915</v>
       </c>
       <c r="E63">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="2">
-        <f>HYPERLINK("pathways/Transfer_of_Acetyl_Groups_into_Mitochondria.csv","Transfer of Acetyl Groups into Mitochondria")</f>
+        <f>HYPERLINK("pathways/Arginine_and_Proline_Metabolism.csv","Arginine and Proline Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B64">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C64">
         <v>-1</v>
       </c>
       <c r="D64">
-        <v>0.987</v>
+        <v>0.92</v>
       </c>
       <c r="E64">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2">
-        <f>HYPERLINK("pathways/Glycine_and_Serine_Metabolism.csv","Glycine and Serine Metabolism")</f>
+        <f>HYPERLINK("pathways/Methionine_Metabolism.csv","Methionine Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B65">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C65">
         <v>-1</v>
       </c>
       <c r="D65">
-        <v>0.991</v>
+        <v>0.925</v>
       </c>
       <c r="E65">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2">
-        <f>HYPERLINK("pathways/Catecholamine_Biosynthesis.csv","Catecholamine Biosynthesis")</f>
+        <f>HYPERLINK("pathways/Degradation_of_Superoxides.csv","Degradation of Superoxides")</f>
         <v>0</v>
       </c>
       <c r="B66">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C66">
         <v>-1</v>
       </c>
       <c r="D66">
-        <v>0.993</v>
+        <v>0.942</v>
       </c>
       <c r="E66">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="2">
-        <f>HYPERLINK("pathways/Glucose_Alanine_Cycle.csv","Glucose-Alanine Cycle")</f>
+        <f>HYPERLINK("pathways/Carnitine_Synthesis.csv","Carnitine Synthesis")</f>
         <v>0</v>
       </c>
       <c r="B67">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C67">
         <v>-1</v>
       </c>
       <c r="D67">
-        <v>0.994</v>
+        <v>0.954</v>
       </c>
       <c r="E67">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="68">
@@ -1588,10 +1588,10 @@
         <v>-1</v>
       </c>
       <c r="D68">
-        <v>0.997</v>
+        <v>0.963</v>
       </c>
       <c r="E68">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="69">
@@ -1606,82 +1606,64 @@
         <v>-1</v>
       </c>
       <c r="D69">
-        <v>0.997</v>
+        <v>0.964</v>
       </c>
       <c r="E69">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="2">
-        <f>HYPERLINK("pathways/Pyruvate_Metabolism.csv","Pyruvate Metabolism")</f>
+        <f>HYPERLINK("pathways/Fatty_Acid_Biosynthesis.csv","Fatty Acid Biosynthesis")</f>
         <v>0</v>
       </c>
       <c r="B70">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C70">
         <v>-1</v>
       </c>
       <c r="D70">
-        <v>0.999</v>
+        <v>0.98</v>
       </c>
       <c r="E70">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="2">
-        <f>HYPERLINK("pathways/Alpha_Linolenic_Acid_and_Linoleic_Acid_Metabolism.csv","Alpha Linolenic Acid and Linoleic Acid Metabolism")</f>
+        <f>HYPERLINK("pathways/Glycine_and_Serine_Metabolism.csv","Glycine and Serine Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B71">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C71">
         <v>-1</v>
       </c>
       <c r="D71">
-        <v>0.999</v>
+        <v>0.985</v>
       </c>
       <c r="E71">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="2">
-        <f>HYPERLINK("pathways/Oxidation_of_Branched_Chain_Fatty_Acids.csv","Oxidation of Branched Chain Fatty Acids")</f>
+        <f>HYPERLINK("pathways/Alpha_Linolenic_Acid_and_Linoleic_Acid_Metabolism.csv","Alpha Linolenic Acid and Linoleic Acid Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B72">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C72">
         <v>-1</v>
       </c>
       <c r="D72">
-        <v>0.999</v>
+        <v>0.988</v>
       </c>
       <c r="E72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" s="2">
-        <f>HYPERLINK("pathways/Fatty_Acid_Biosynthesis.csv","Fatty Acid Biosynthesis")</f>
-        <v>0</v>
-      </c>
-      <c r="B73">
-        <v>9</v>
-      </c>
-      <c r="C73">
-        <v>-1</v>
-      </c>
-      <c r="D73">
-        <v>1</v>
-      </c>
-      <c r="E73">
-        <v>1</v>
+        <v>0.988</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
uploading manuscript to biorxiv
</commit_message>
<xml_diff>
--- a/results/dins30_cameraPR/dins30_cameraPR.xlsx
+++ b/results/dins30_cameraPR/dins30_cameraPR.xlsx
@@ -400,10 +400,10 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>3.74e-007</v>
+        <v>2.4e-007</v>
       </c>
       <c r="E2">
-        <v>2.66e-005</v>
+        <v>1.7e-005</v>
       </c>
     </row>
     <row r="3">
@@ -418,10 +418,10 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0.0509</v>
+        <v>0.0679</v>
       </c>
       <c r="E3">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="4">
@@ -436,10 +436,10 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>0.08989999999999999</v>
+        <v>0.105</v>
       </c>
       <c r="E4">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="5">
@@ -454,10 +454,10 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>0.117</v>
+        <v>0.121</v>
       </c>
       <c r="E5">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="6">
@@ -472,10 +472,10 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>0.127</v>
+        <v>0.149</v>
       </c>
       <c r="E6">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="7">
@@ -490,10 +490,10 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>0.168</v>
+        <v>0.195</v>
       </c>
       <c r="E7">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="8">
@@ -508,10 +508,10 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>0.182</v>
+        <v>0.219</v>
       </c>
       <c r="E8">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="9">
@@ -526,10 +526,10 @@
         <v>1</v>
       </c>
       <c r="D9">
-        <v>0.229</v>
+        <v>0.262</v>
       </c>
       <c r="E9">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="10">
@@ -544,46 +544,46 @@
         <v>1</v>
       </c>
       <c r="D10">
-        <v>0.323</v>
+        <v>0.322</v>
       </c>
       <c r="E10">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2">
-        <f>HYPERLINK("pathways/Nicotinate_and_Nicotinamide_Metabolism.csv","Nicotinate and Nicotinamide Metabolism")</f>
+        <f>HYPERLINK("pathways/Phosphatidylinositol_Phosphate_Metabolism.csv","Phosphatidylinositol Phosphate Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B11">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11">
-        <v>0.34</v>
+        <v>0.379</v>
       </c>
       <c r="E11">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2">
-        <f>HYPERLINK("pathways/Phosphatidylinositol_Phosphate_Metabolism.csv","Phosphatidylinositol Phosphate Metabolism")</f>
+        <f>HYPERLINK("pathways/Nicotinate_and_Nicotinamide_Metabolism.csv","Nicotinate and Nicotinamide Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12">
-        <v>0.342</v>
+        <v>0.389</v>
       </c>
       <c r="E12">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="13">
@@ -598,10 +598,10 @@
         <v>1</v>
       </c>
       <c r="D13">
-        <v>0.422</v>
+        <v>0.443</v>
       </c>
       <c r="E13">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="14">
@@ -616,51 +616,51 @@
         <v>1</v>
       </c>
       <c r="D14">
-        <v>0.457</v>
+        <v>0.48</v>
       </c>
       <c r="E14">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2">
-        <f>HYPERLINK("pathways/Galactose_Metabolism.csv","Galactose Metabolism")</f>
+        <f>HYPERLINK("pathways/Lactose_Synthesis.csv","Lactose Synthesis")</f>
         <v>0</v>
       </c>
       <c r="B15">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15">
-        <v>0.462</v>
+        <v>0.496</v>
       </c>
       <c r="E15">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2">
-        <f>HYPERLINK("pathways/Cysteine_Metabolism.csv","Cysteine Metabolism")</f>
+        <f>HYPERLINK("pathways/Galactose_Metabolism.csv","Galactose Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B16">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16">
         <v>-1</v>
       </c>
       <c r="D16">
-        <v>0.501</v>
+        <v>0.521</v>
       </c>
       <c r="E16">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2">
-        <f>HYPERLINK("pathways/Methylhistidine_Metabolism.csv","Methylhistidine Metabolism")</f>
+        <f>HYPERLINK("pathways/Glycerol_Phosphate_Shuttle.csv","Glycerol Phosphate Shuttle")</f>
         <v>0</v>
       </c>
       <c r="B17">
@@ -670,28 +670,28 @@
         <v>-1</v>
       </c>
       <c r="D17">
-        <v>0.52</v>
+        <v>0.566</v>
       </c>
       <c r="E17">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2">
-        <f>HYPERLINK("pathways/Lactose_Synthesis.csv","Lactose Synthesis")</f>
+        <f>HYPERLINK("pathways/Cysteine_Metabolism.csv","Cysteine Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C18">
         <v>-1</v>
       </c>
       <c r="D18">
-        <v>0.529</v>
+        <v>0.578</v>
       </c>
       <c r="E18">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="19">
@@ -706,15 +706,15 @@
         <v>-1</v>
       </c>
       <c r="D19">
-        <v>0.542</v>
+        <v>0.578</v>
       </c>
       <c r="E19">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2">
-        <f>HYPERLINK("pathways/Glycerol_Phosphate_Shuttle.csv","Glycerol Phosphate Shuttle")</f>
+        <f>HYPERLINK("pathways/Methylhistidine_Metabolism.csv","Methylhistidine Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B20">
@@ -724,10 +724,10 @@
         <v>-1</v>
       </c>
       <c r="D20">
-        <v>0.542</v>
+        <v>0.581</v>
       </c>
       <c r="E20">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="21">
@@ -742,123 +742,123 @@
         <v>-1</v>
       </c>
       <c r="D21">
-        <v>0.546</v>
+        <v>0.589</v>
       </c>
       <c r="E21">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2">
-        <f>HYPERLINK("pathways/Histidine_Metabolism.csv","Histidine Metabolism")</f>
+        <f>HYPERLINK("pathways/Sulfate_Sulfite_Metabolism.csv","Sulfate/Sulfite Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B22">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C22">
         <v>-1</v>
       </c>
       <c r="D22">
-        <v>0.5620000000000001</v>
+        <v>0.626</v>
       </c>
       <c r="E22">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2">
-        <f>HYPERLINK("pathways/Sulfate_Sulfite_Metabolism.csv","Sulfate/Sulfite Metabolism")</f>
+        <f>HYPERLINK("pathways/Histidine_Metabolism.csv","Histidine Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B23">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C23">
         <v>-1</v>
       </c>
       <c r="D23">
-        <v>0.574</v>
+        <v>0.637</v>
       </c>
       <c r="E23">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2">
-        <f>HYPERLINK("pathways/Warburg_Effect.csv","Warburg Effect")</f>
+        <f>HYPERLINK("pathways/Pyrimidine_Metabolism.csv","Pyrimidine Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B24">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C24">
         <v>-1</v>
       </c>
       <c r="D24">
-        <v>0.641</v>
+        <v>0.645</v>
       </c>
       <c r="E24">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2">
-        <f>HYPERLINK("pathways/Pyrimidine_Metabolism.csv","Pyrimidine Metabolism")</f>
+        <f>HYPERLINK("pathways/Bile_Acid_Biosynthesis.csv","Bile Acid Biosynthesis")</f>
         <v>0</v>
       </c>
       <c r="B25">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C25">
         <v>-1</v>
       </c>
       <c r="D25">
-        <v>0.646</v>
+        <v>0.648</v>
       </c>
       <c r="E25">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2">
-        <f>HYPERLINK("pathways/Bile_Acid_Biosynthesis.csv","Bile Acid Biosynthesis")</f>
+        <f>HYPERLINK("pathways/Selenoamino_Acid_Metabolism.csv","Selenoamino Acid Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B26">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C26">
         <v>-1</v>
       </c>
       <c r="D26">
-        <v>0.648</v>
+        <v>0.693</v>
       </c>
       <c r="E26">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2">
-        <f>HYPERLINK("pathways/Selenoamino_Acid_Metabolism.csv","Selenoamino Acid Metabolism")</f>
+        <f>HYPERLINK("pathways/Aspartate_Metabolism.csv","Aspartate Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B27">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C27">
         <v>-1</v>
       </c>
       <c r="D27">
-        <v>0.655</v>
+        <v>0.704</v>
       </c>
       <c r="E27">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2">
-        <f>HYPERLINK("pathways/Butyrate_Metabolism.csv","Butyrate Metabolism")</f>
+        <f>HYPERLINK("pathways/Pantothenate_and_CoA_Biosynthesis.csv","Pantothenate and CoA Biosynthesis")</f>
         <v>0</v>
       </c>
       <c r="B28">
@@ -868,231 +868,231 @@
         <v>-1</v>
       </c>
       <c r="D28">
-        <v>0.701</v>
+        <v>0.72</v>
       </c>
       <c r="E28">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2">
-        <f>HYPERLINK("pathways/Ethanol_Degradation.csv","Ethanol Degradation")</f>
+        <f>HYPERLINK("pathways/Ammonia_Recycling.csv","Ammonia Recycling")</f>
         <v>0</v>
       </c>
       <c r="B29">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C29">
         <v>-1</v>
       </c>
       <c r="D29">
-        <v>0.701</v>
+        <v>0.727</v>
       </c>
       <c r="E29">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2">
-        <f>HYPERLINK("pathways/Pantothenate_and_CoA_Biosynthesis.csv","Pantothenate and CoA Biosynthesis")</f>
+        <f>HYPERLINK("pathways/Warburg_Effect.csv","Warburg Effect")</f>
         <v>0</v>
       </c>
       <c r="B30">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C30">
         <v>-1</v>
       </c>
       <c r="D30">
-        <v>0.701</v>
+        <v>0.733</v>
       </c>
       <c r="E30">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2">
-        <f>HYPERLINK("pathways/Tryptophan_Metabolism.csv","Tryptophan Metabolism")</f>
+        <f>HYPERLINK("pathways/Malate_Aspartate_Shuttle.csv","Malate-Aspartate Shuttle")</f>
         <v>0</v>
       </c>
       <c r="B31">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C31">
         <v>-1</v>
       </c>
       <c r="D31">
-        <v>0.712</v>
+        <v>0.758</v>
       </c>
       <c r="E31">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2">
-        <f>HYPERLINK("pathways/Glycolysis.csv","Glycolysis")</f>
+        <f>HYPERLINK("pathways/Propanoate_Metabolism.csv","Propanoate Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B32">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C32">
         <v>-1</v>
       </c>
       <c r="D32">
-        <v>0.715</v>
+        <v>0.76</v>
       </c>
       <c r="E32">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2">
-        <f>HYPERLINK("pathways/Androgen_and_Estrogen_Metabolism.csv","Androgen and Estrogen Metabolism")</f>
+        <f>HYPERLINK("pathways/Butyrate_Metabolism.csv","Butyrate Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C33">
         <v>-1</v>
       </c>
       <c r="D33">
-        <v>0.718</v>
+        <v>0.761</v>
       </c>
       <c r="E33">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2">
-        <f>HYPERLINK("pathways/Arachidonic_Acid_Metabolism.csv","Arachidonic Acid Metabolism")</f>
+        <f>HYPERLINK("pathways/Ethanol_Degradation.csv","Ethanol Degradation")</f>
         <v>0</v>
       </c>
       <c r="B34">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C34">
         <v>-1</v>
       </c>
       <c r="D34">
-        <v>0.733</v>
+        <v>0.763</v>
       </c>
       <c r="E34">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2">
-        <f>HYPERLINK("pathways/Ammonia_Recycling.csv","Ammonia Recycling")</f>
+        <f>HYPERLINK("pathways/Glycolysis.csv","Glycolysis")</f>
         <v>0</v>
       </c>
       <c r="B35">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C35">
         <v>-1</v>
       </c>
       <c r="D35">
-        <v>0.738</v>
+        <v>0.765</v>
       </c>
       <c r="E35">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2">
-        <f>HYPERLINK("pathways/Aspartate_Metabolism.csv","Aspartate Metabolism")</f>
+        <f>HYPERLINK("pathways/Arachidonic_Acid_Metabolism.csv","Arachidonic Acid Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B36">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C36">
         <v>-1</v>
       </c>
       <c r="D36">
-        <v>0.739</v>
+        <v>0.776</v>
       </c>
       <c r="E36">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2">
-        <f>HYPERLINK("pathways/Propanoate_Metabolism.csv","Propanoate Metabolism")</f>
+        <f>HYPERLINK("pathways/Riboflavin_Metabolism.csv","Riboflavin Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B37">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C37">
         <v>-1</v>
       </c>
       <c r="D37">
-        <v>0.743</v>
+        <v>0.786</v>
       </c>
       <c r="E37">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2">
-        <f>HYPERLINK("pathways/Malate_Aspartate_Shuttle.csv","Malate-Aspartate Shuttle")</f>
+        <f>HYPERLINK("pathways/Androgen_and_Estrogen_Metabolism.csv","Androgen and Estrogen Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B38">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C38">
         <v>-1</v>
       </c>
       <c r="D38">
-        <v>0.782</v>
+        <v>0.794</v>
       </c>
       <c r="E38">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2">
-        <f>HYPERLINK("pathways/Riboflavin_Metabolism.csv","Riboflavin Metabolism")</f>
+        <f>HYPERLINK("pathways/Tryptophan_Metabolism.csv","Tryptophan Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B39">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C39">
         <v>-1</v>
       </c>
       <c r="D39">
-        <v>0.8010000000000001</v>
+        <v>0.8</v>
       </c>
       <c r="E39">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2">
-        <f>HYPERLINK("pathways/Homocysteine_Degradation.csv","Homocysteine Degradation")</f>
+        <f>HYPERLINK("pathways/Purine_Metabolism.csv","Purine Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B40">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C40">
         <v>-1</v>
       </c>
       <c r="D40">
-        <v>0.8090000000000001</v>
+        <v>0.82</v>
       </c>
       <c r="E40">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2">
-        <f>HYPERLINK("pathways/Spermidine_and_Spermine_Biosynthesis.csv","Spermidine and Spermine Biosynthesis")</f>
+        <f>HYPERLINK("pathways/Homocysteine_Degradation.csv","Homocysteine Degradation")</f>
         <v>0</v>
       </c>
       <c r="B41">
@@ -1102,249 +1102,249 @@
         <v>-1</v>
       </c>
       <c r="D41">
-        <v>0.832</v>
+        <v>0.826</v>
       </c>
       <c r="E41">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2">
-        <f>HYPERLINK("pathways/Steroid_Biosynthesis.csv","Steroid Biosynthesis")</f>
+        <f>HYPERLINK("pathways/Spermidine_and_Spermine_Biosynthesis.csv","Spermidine and Spermine Biosynthesis")</f>
         <v>0</v>
       </c>
       <c r="B42">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C42">
         <v>-1</v>
       </c>
       <c r="D42">
-        <v>0.835</v>
+        <v>0.834</v>
       </c>
       <c r="E42">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2">
-        <f>HYPERLINK("pathways/Gluconeogenesis.csv","Gluconeogenesis")</f>
+        <f>HYPERLINK("pathways/Betaine_Metabolism.csv","Betaine Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B43">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C43">
         <v>-1</v>
       </c>
       <c r="D43">
-        <v>0.836</v>
+        <v>0.851</v>
       </c>
       <c r="E43">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2">
-        <f>HYPERLINK("pathways/Betaine_Metabolism.csv","Betaine Metabolism")</f>
+        <f>HYPERLINK("pathways/Vitamin_B6_Metabolism.csv","Vitamin B6 Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B44">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C44">
         <v>-1</v>
       </c>
       <c r="D44">
-        <v>0.842</v>
+        <v>0.857</v>
       </c>
       <c r="E44">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2">
-        <f>HYPERLINK("pathways/Vitamin_B6_Metabolism.csv","Vitamin B6 Metabolism")</f>
+        <f>HYPERLINK("pathways/Glycerolipid_Metabolism.csv","Glycerolipid Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B45">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C45">
         <v>-1</v>
       </c>
       <c r="D45">
-        <v>0.847</v>
+        <v>0.858</v>
       </c>
       <c r="E45">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2">
-        <f>HYPERLINK("pathways/Glucose_Alanine_Cycle.csv","Glucose-Alanine Cycle")</f>
+        <f>HYPERLINK("pathways/Glutathione_Metabolism.csv","Glutathione Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B46">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C46">
         <v>-1</v>
       </c>
       <c r="D46">
-        <v>0.85</v>
+        <v>0.861</v>
       </c>
       <c r="E46">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2">
-        <f>HYPERLINK("pathways/Purine_Metabolism.csv","Purine Metabolism")</f>
+        <f>HYPERLINK("pathways/Steroid_Biosynthesis.csv","Steroid Biosynthesis")</f>
         <v>0</v>
       </c>
       <c r="B47">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C47">
         <v>-1</v>
       </c>
       <c r="D47">
-        <v>0.852</v>
+        <v>0.87</v>
       </c>
       <c r="E47">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2">
-        <f>HYPERLINK("pathways/Glycerolipid_Metabolism.csv","Glycerolipid Metabolism")</f>
+        <f>HYPERLINK("pathways/Gluconeogenesis.csv","Gluconeogenesis")</f>
         <v>0</v>
       </c>
       <c r="B48">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C48">
         <v>-1</v>
       </c>
       <c r="D48">
-        <v>0.854</v>
+        <v>0.881</v>
       </c>
       <c r="E48">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2">
-        <f>HYPERLINK("pathways/Glutathione_Metabolism.csv","Glutathione Metabolism")</f>
+        <f>HYPERLINK("pathways/Starch_and_Sucrose_Metabolism.csv","Starch and Sucrose Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B49">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C49">
         <v>-1</v>
       </c>
       <c r="D49">
-        <v>0.856</v>
+        <v>0.881</v>
       </c>
       <c r="E49">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2">
-        <f>HYPERLINK("pathways/Urea_Cycle.csv","Urea Cycle")</f>
+        <f>HYPERLINK("pathways/Porphyrin_Metabolism.csv","Porphyrin Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B50">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C50">
         <v>-1</v>
       </c>
       <c r="D50">
-        <v>0.866</v>
+        <v>0.883</v>
       </c>
       <c r="E50">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2">
-        <f>HYPERLINK("pathways/Starch_and_Sucrose_Metabolism.csv","Starch and Sucrose Metabolism")</f>
+        <f>HYPERLINK("pathways/Urea_Cycle.csv","Urea Cycle")</f>
         <v>0</v>
       </c>
       <c r="B51">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C51">
         <v>-1</v>
       </c>
       <c r="D51">
-        <v>0.867</v>
+        <v>0.891</v>
       </c>
       <c r="E51">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2">
-        <f>HYPERLINK("pathways/Porphyrin_Metabolism.csv","Porphyrin Metabolism")</f>
+        <f>HYPERLINK("pathways/Glucose_Alanine_Cycle.csv","Glucose-Alanine Cycle")</f>
         <v>0</v>
       </c>
       <c r="B52">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C52">
         <v>-1</v>
       </c>
       <c r="D52">
-        <v>0.889</v>
+        <v>0.9</v>
       </c>
       <c r="E52">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2">
-        <f>HYPERLINK("pathways/Mitochondrial_Electron_Transport_Chain.csv","Mitochondrial Electron Transport Chain")</f>
+        <f>HYPERLINK("pathways/Tyrosine_Metabolism.csv","Tyrosine Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B53">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C53">
         <v>-1</v>
       </c>
       <c r="D53">
-        <v>0.889</v>
+        <v>0.902</v>
       </c>
       <c r="E53">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2">
-        <f>HYPERLINK("pathways/Tyrosine_Metabolism.csv","Tyrosine Metabolism")</f>
+        <f>HYPERLINK("pathways/Alanine_Metabolism.csv","Alanine Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B54">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C54">
         <v>-1</v>
       </c>
       <c r="D54">
-        <v>0.9</v>
+        <v>0.915</v>
       </c>
       <c r="E54">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2">
-        <f>HYPERLINK("pathways/Thyroid_hormone_synthesis.csv","Thyroid hormone synthesis")</f>
+        <f>HYPERLINK("pathways/Lysine_Degradation.csv","Lysine Degradation")</f>
         <v>0</v>
       </c>
       <c r="B55">
@@ -1354,123 +1354,123 @@
         <v>-1</v>
       </c>
       <c r="D55">
-        <v>0.901</v>
+        <v>0.918</v>
       </c>
       <c r="E55">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2">
-        <f>HYPERLINK("pathways/Alanine_Metabolism.csv","Alanine Metabolism")</f>
+        <f>HYPERLINK("pathways/Methionine_Metabolism.csv","Methionine Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B56">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C56">
         <v>-1</v>
       </c>
       <c r="D56">
-        <v>0.902</v>
+        <v>0.919</v>
       </c>
       <c r="E56">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2">
-        <f>HYPERLINK("pathways/Lysine_Degradation.csv","Lysine Degradation")</f>
+        <f>HYPERLINK("pathways/Mitochondrial_Electron_Transport_Chain.csv","Mitochondrial Electron Transport Chain")</f>
         <v>0</v>
       </c>
       <c r="B57">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C57">
         <v>-1</v>
       </c>
       <c r="D57">
-        <v>0.902</v>
+        <v>0.92</v>
       </c>
       <c r="E57">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2">
-        <f>HYPERLINK("pathways/Glutamate_Metabolism.csv","Glutamate Metabolism")</f>
+        <f>HYPERLINK("pathways/Arginine_and_Proline_Metabolism.csv","Arginine and Proline Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B58">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C58">
         <v>-1</v>
       </c>
       <c r="D58">
-        <v>0.902</v>
+        <v>0.924</v>
       </c>
       <c r="E58">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2">
-        <f>HYPERLINK("pathways/Pyruvate_Metabolism.csv","Pyruvate Metabolism")</f>
+        <f>HYPERLINK("pathways/Glutamate_Metabolism.csv","Glutamate Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B59">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C59">
         <v>-1</v>
       </c>
       <c r="D59">
-        <v>0.905</v>
+        <v>0.9260000000000001</v>
       </c>
       <c r="E59">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2">
-        <f>HYPERLINK("pathways/Transfer_of_Acetyl_Groups_into_Mitochondria.csv","Transfer of Acetyl Groups into Mitochondria")</f>
+        <f>HYPERLINK("pathways/Degradation_of_Superoxides.csv","Degradation of Superoxides")</f>
         <v>0</v>
       </c>
       <c r="B60">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C60">
         <v>-1</v>
       </c>
       <c r="D60">
-        <v>0.91</v>
+        <v>0.9290000000000001</v>
       </c>
       <c r="E60">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="2">
-        <f>HYPERLINK("pathways/Catecholamine_Biosynthesis.csv","Catecholamine Biosynthesis")</f>
+        <f>HYPERLINK("pathways/Transfer_of_Acetyl_Groups_into_Mitochondria.csv","Transfer of Acetyl Groups into Mitochondria")</f>
         <v>0</v>
       </c>
       <c r="B61">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C61">
         <v>-1</v>
       </c>
       <c r="D61">
-        <v>0.915</v>
+        <v>0.9300000000000001</v>
       </c>
       <c r="E61">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="2">
-        <f>HYPERLINK("pathways/Oxidation_of_Branched_Chain_Fatty_Acids.csv","Oxidation of Branched Chain Fatty Acids")</f>
+        <f>HYPERLINK("pathways/Catecholamine_Biosynthesis.csv","Catecholamine Biosynthesis")</f>
         <v>0</v>
       </c>
       <c r="B62">
@@ -1480,82 +1480,82 @@
         <v>-1</v>
       </c>
       <c r="D62">
-        <v>0.915</v>
+        <v>0.9300000000000001</v>
       </c>
       <c r="E62">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="2">
-        <f>HYPERLINK("pathways/Steroidogenesis.csv","Steroidogenesis")</f>
+        <f>HYPERLINK("pathways/Pyruvate_Metabolism.csv","Pyruvate Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B63">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C63">
         <v>-1</v>
       </c>
       <c r="D63">
-        <v>0.915</v>
+        <v>0.9310000000000001</v>
       </c>
       <c r="E63">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="2">
-        <f>HYPERLINK("pathways/Arginine_and_Proline_Metabolism.csv","Arginine and Proline Metabolism")</f>
+        <f>HYPERLINK("pathways/Thyroid_hormone_synthesis.csv","Thyroid hormone synthesis")</f>
         <v>0</v>
       </c>
       <c r="B64">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C64">
         <v>-1</v>
       </c>
       <c r="D64">
-        <v>0.92</v>
+        <v>0.9320000000000001</v>
       </c>
       <c r="E64">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2">
-        <f>HYPERLINK("pathways/Methionine_Metabolism.csv","Methionine Metabolism")</f>
+        <f>HYPERLINK("pathways/Steroidogenesis.csv","Steroidogenesis")</f>
         <v>0</v>
       </c>
       <c r="B65">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C65">
         <v>-1</v>
       </c>
       <c r="D65">
-        <v>0.925</v>
+        <v>0.9350000000000001</v>
       </c>
       <c r="E65">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2">
-        <f>HYPERLINK("pathways/Degradation_of_Superoxides.csv","Degradation of Superoxides")</f>
+        <f>HYPERLINK("pathways/Oxidation_of_Branched_Chain_Fatty_Acids.csv","Oxidation of Branched Chain Fatty Acids")</f>
         <v>0</v>
       </c>
       <c r="B66">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C66">
         <v>-1</v>
       </c>
       <c r="D66">
-        <v>0.942</v>
+        <v>0.941</v>
       </c>
       <c r="E66">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="67">
@@ -1570,87 +1570,87 @@
         <v>-1</v>
       </c>
       <c r="D67">
-        <v>0.954</v>
+        <v>0.966</v>
       </c>
       <c r="E67">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="2">
-        <f>HYPERLINK("pathways/Citric_Acid_Cycle.csv","Citric Acid Cycle")</f>
+        <f>HYPERLINK("pathways/Valine__Leucine_and_Isoleucine_Degradation.csv","Valine, Leucine and Isoleucine Degradation")</f>
         <v>0</v>
       </c>
       <c r="B68">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C68">
         <v>-1</v>
       </c>
       <c r="D68">
-        <v>0.963</v>
+        <v>0.969</v>
       </c>
       <c r="E68">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="2">
-        <f>HYPERLINK("pathways/Valine__Leucine_and_Isoleucine_Degradation.csv","Valine, Leucine and Isoleucine Degradation")</f>
+        <f>HYPERLINK("pathways/Citric_Acid_Cycle.csv","Citric Acid Cycle")</f>
         <v>0</v>
       </c>
       <c r="B69">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C69">
         <v>-1</v>
       </c>
       <c r="D69">
-        <v>0.964</v>
+        <v>0.979</v>
       </c>
       <c r="E69">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="2">
-        <f>HYPERLINK("pathways/Fatty_Acid_Biosynthesis.csv","Fatty Acid Biosynthesis")</f>
+        <f>HYPERLINK("pathways/Glycine_and_Serine_Metabolism.csv","Glycine and Serine Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B70">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C70">
         <v>-1</v>
       </c>
       <c r="D70">
-        <v>0.98</v>
+        <v>0.983</v>
       </c>
       <c r="E70">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="2">
-        <f>HYPERLINK("pathways/Glycine_and_Serine_Metabolism.csv","Glycine and Serine Metabolism")</f>
+        <f>HYPERLINK("pathways/Alpha_Linolenic_Acid_and_Linoleic_Acid_Metabolism.csv","Alpha Linolenic Acid and Linoleic Acid Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B71">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C71">
         <v>-1</v>
       </c>
       <c r="D71">
-        <v>0.985</v>
+        <v>0.986</v>
       </c>
       <c r="E71">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="2">
-        <f>HYPERLINK("pathways/Alpha_Linolenic_Acid_and_Linoleic_Acid_Metabolism.csv","Alpha Linolenic Acid and Linoleic Acid Metabolism")</f>
+        <f>HYPERLINK("pathways/Fatty_Acid_Biosynthesis.csv","Fatty Acid Biosynthesis")</f>
         <v>0</v>
       </c>
       <c r="B72">
@@ -1660,10 +1660,10 @@
         <v>-1</v>
       </c>
       <c r="D72">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
       <c r="E72">
-        <v>0.988</v>
+        <v>0.989</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
run analyze_slimm_t2d_omics with Hitman with updated limma_pcor
</commit_message>
<xml_diff>
--- a/results/dins30_cameraPR/dins30_cameraPR.xlsx
+++ b/results/dins30_cameraPR/dins30_cameraPR.xlsx
@@ -400,10 +400,10 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>3.74e-007</v>
+        <v>4.18e-007</v>
       </c>
       <c r="E2">
-        <v>2.66e-005</v>
+        <v>2.97e-005</v>
       </c>
     </row>
     <row r="3">
@@ -418,7 +418,7 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0.0509</v>
+        <v>0.051</v>
       </c>
       <c r="E3">
         <v>0.988</v>
@@ -436,7 +436,7 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>0.08989999999999999</v>
+        <v>0.09</v>
       </c>
       <c r="E4">
         <v>0.988</v>
@@ -454,7 +454,7 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>0.117</v>
+        <v>0.11</v>
       </c>
       <c r="E5">
         <v>0.988</v>
@@ -472,7 +472,7 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>0.127</v>
+        <v>0.128</v>
       </c>
       <c r="E6">
         <v>0.988</v>
@@ -490,7 +490,7 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>0.168</v>
+        <v>0.172</v>
       </c>
       <c r="E7">
         <v>0.988</v>
@@ -508,7 +508,7 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>0.182</v>
+        <v>0.175</v>
       </c>
       <c r="E8">
         <v>0.988</v>
@@ -526,7 +526,7 @@
         <v>1</v>
       </c>
       <c r="D9">
-        <v>0.229</v>
+        <v>0.228</v>
       </c>
       <c r="E9">
         <v>0.988</v>
@@ -544,7 +544,7 @@
         <v>1</v>
       </c>
       <c r="D10">
-        <v>0.323</v>
+        <v>0.326</v>
       </c>
       <c r="E10">
         <v>0.988</v>
@@ -562,7 +562,7 @@
         <v>1</v>
       </c>
       <c r="D11">
-        <v>0.34</v>
+        <v>0.331</v>
       </c>
       <c r="E11">
         <v>0.988</v>
@@ -580,7 +580,7 @@
         <v>1</v>
       </c>
       <c r="D12">
-        <v>0.342</v>
+        <v>0.337</v>
       </c>
       <c r="E12">
         <v>0.988</v>
@@ -598,7 +598,7 @@
         <v>1</v>
       </c>
       <c r="D13">
-        <v>0.422</v>
+        <v>0.417</v>
       </c>
       <c r="E13">
         <v>0.988</v>
@@ -616,7 +616,7 @@
         <v>1</v>
       </c>
       <c r="D14">
-        <v>0.457</v>
+        <v>0.448</v>
       </c>
       <c r="E14">
         <v>0.988</v>
@@ -634,7 +634,7 @@
         <v>1</v>
       </c>
       <c r="D15">
-        <v>0.462</v>
+        <v>0.455</v>
       </c>
       <c r="E15">
         <v>0.988</v>
@@ -649,10 +649,10 @@
         <v>7</v>
       </c>
       <c r="C16">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <v>0.501</v>
+        <v>0.498</v>
       </c>
       <c r="E16">
         <v>0.988</v>
@@ -670,7 +670,7 @@
         <v>-1</v>
       </c>
       <c r="D17">
-        <v>0.52</v>
+        <v>0.519</v>
       </c>
       <c r="E17">
         <v>0.988</v>
@@ -688,7 +688,7 @@
         <v>-1</v>
       </c>
       <c r="D18">
-        <v>0.529</v>
+        <v>0.533</v>
       </c>
       <c r="E18">
         <v>0.988</v>
@@ -696,17 +696,17 @@
     </row>
     <row r="19">
       <c r="A19" s="2">
-        <f>HYPERLINK("pathways/Beta_Alanine_Metabolism.csv","Beta-Alanine Metabolism")</f>
+        <f>HYPERLINK("pathways/Glycerol_Phosphate_Shuttle.csv","Glycerol Phosphate Shuttle")</f>
         <v>0</v>
       </c>
       <c r="B19">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C19">
         <v>-1</v>
       </c>
       <c r="D19">
-        <v>0.542</v>
+        <v>0.538</v>
       </c>
       <c r="E19">
         <v>0.988</v>
@@ -714,17 +714,17 @@
     </row>
     <row r="20">
       <c r="A20" s="2">
-        <f>HYPERLINK("pathways/Glycerol_Phosphate_Shuttle.csv","Glycerol Phosphate Shuttle")</f>
+        <f>HYPERLINK("pathways/Beta_Alanine_Metabolism.csv","Beta-Alanine Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C20">
         <v>-1</v>
       </c>
       <c r="D20">
-        <v>0.542</v>
+        <v>0.538</v>
       </c>
       <c r="E20">
         <v>0.988</v>
@@ -742,7 +742,7 @@
         <v>-1</v>
       </c>
       <c r="D21">
-        <v>0.546</v>
+        <v>0.543</v>
       </c>
       <c r="E21">
         <v>0.988</v>
@@ -760,7 +760,7 @@
         <v>-1</v>
       </c>
       <c r="D22">
-        <v>0.5620000000000001</v>
+        <v>0.5590000000000001</v>
       </c>
       <c r="E22">
         <v>0.988</v>
@@ -778,7 +778,7 @@
         <v>-1</v>
       </c>
       <c r="D23">
-        <v>0.574</v>
+        <v>0.569</v>
       </c>
       <c r="E23">
         <v>0.988</v>
@@ -786,17 +786,17 @@
     </row>
     <row r="24">
       <c r="A24" s="2">
-        <f>HYPERLINK("pathways/Warburg_Effect.csv","Warburg Effect")</f>
+        <f>HYPERLINK("pathways/Pyrimidine_Metabolism.csv","Pyrimidine Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B24">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C24">
         <v>-1</v>
       </c>
       <c r="D24">
-        <v>0.641</v>
+        <v>0.64</v>
       </c>
       <c r="E24">
         <v>0.988</v>
@@ -804,17 +804,17 @@
     </row>
     <row r="25">
       <c r="A25" s="2">
-        <f>HYPERLINK("pathways/Pyrimidine_Metabolism.csv","Pyrimidine Metabolism")</f>
+        <f>HYPERLINK("pathways/Warburg_Effect.csv","Warburg Effect")</f>
         <v>0</v>
       </c>
       <c r="B25">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C25">
         <v>-1</v>
       </c>
       <c r="D25">
-        <v>0.646</v>
+        <v>0.64</v>
       </c>
       <c r="E25">
         <v>0.988</v>
@@ -832,7 +832,7 @@
         <v>-1</v>
       </c>
       <c r="D26">
-        <v>0.648</v>
+        <v>0.652</v>
       </c>
       <c r="E26">
         <v>0.988</v>
@@ -850,7 +850,7 @@
         <v>-1</v>
       </c>
       <c r="D27">
-        <v>0.655</v>
+        <v>0.654</v>
       </c>
       <c r="E27">
         <v>0.988</v>
@@ -868,7 +868,7 @@
         <v>-1</v>
       </c>
       <c r="D28">
-        <v>0.701</v>
+        <v>0.698</v>
       </c>
       <c r="E28">
         <v>0.988</v>
@@ -886,7 +886,7 @@
         <v>-1</v>
       </c>
       <c r="D29">
-        <v>0.701</v>
+        <v>0.698</v>
       </c>
       <c r="E29">
         <v>0.988</v>
@@ -904,7 +904,7 @@
         <v>-1</v>
       </c>
       <c r="D30">
-        <v>0.701</v>
+        <v>0.698</v>
       </c>
       <c r="E30">
         <v>0.988</v>
@@ -922,7 +922,7 @@
         <v>-1</v>
       </c>
       <c r="D31">
-        <v>0.712</v>
+        <v>0.71</v>
       </c>
       <c r="E31">
         <v>0.988</v>
@@ -940,7 +940,7 @@
         <v>-1</v>
       </c>
       <c r="D32">
-        <v>0.715</v>
+        <v>0.712</v>
       </c>
       <c r="E32">
         <v>0.988</v>
@@ -958,7 +958,7 @@
         <v>-1</v>
       </c>
       <c r="D33">
-        <v>0.718</v>
+        <v>0.716</v>
       </c>
       <c r="E33">
         <v>0.988</v>
@@ -976,7 +976,7 @@
         <v>-1</v>
       </c>
       <c r="D34">
-        <v>0.733</v>
+        <v>0.734</v>
       </c>
       <c r="E34">
         <v>0.988</v>
@@ -994,7 +994,7 @@
         <v>-1</v>
       </c>
       <c r="D35">
-        <v>0.738</v>
+        <v>0.734</v>
       </c>
       <c r="E35">
         <v>0.988</v>
@@ -1030,7 +1030,7 @@
         <v>-1</v>
       </c>
       <c r="D37">
-        <v>0.743</v>
+        <v>0.742</v>
       </c>
       <c r="E37">
         <v>0.988</v>
@@ -1048,7 +1048,7 @@
         <v>-1</v>
       </c>
       <c r="D38">
-        <v>0.782</v>
+        <v>0.783</v>
       </c>
       <c r="E38">
         <v>0.988</v>
@@ -1066,7 +1066,7 @@
         <v>-1</v>
       </c>
       <c r="D39">
-        <v>0.8010000000000001</v>
+        <v>0.799</v>
       </c>
       <c r="E39">
         <v>0.988</v>
@@ -1084,7 +1084,7 @@
         <v>-1</v>
       </c>
       <c r="D40">
-        <v>0.8090000000000001</v>
+        <v>0.8080000000000001</v>
       </c>
       <c r="E40">
         <v>0.988</v>
@@ -1110,17 +1110,17 @@
     </row>
     <row r="42">
       <c r="A42" s="2">
-        <f>HYPERLINK("pathways/Steroid_Biosynthesis.csv","Steroid Biosynthesis")</f>
+        <f>HYPERLINK("pathways/Gluconeogenesis.csv","Gluconeogenesis")</f>
         <v>0</v>
       </c>
       <c r="B42">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C42">
         <v>-1</v>
       </c>
       <c r="D42">
-        <v>0.835</v>
+        <v>0.833</v>
       </c>
       <c r="E42">
         <v>0.988</v>
@@ -1128,17 +1128,17 @@
     </row>
     <row r="43">
       <c r="A43" s="2">
-        <f>HYPERLINK("pathways/Gluconeogenesis.csv","Gluconeogenesis")</f>
+        <f>HYPERLINK("pathways/Steroid_Biosynthesis.csv","Steroid Biosynthesis")</f>
         <v>0</v>
       </c>
       <c r="B43">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C43">
         <v>-1</v>
       </c>
       <c r="D43">
-        <v>0.836</v>
+        <v>0.835</v>
       </c>
       <c r="E43">
         <v>0.988</v>
@@ -1156,7 +1156,7 @@
         <v>-1</v>
       </c>
       <c r="D44">
-        <v>0.842</v>
+        <v>0.843</v>
       </c>
       <c r="E44">
         <v>0.988</v>
@@ -1210,7 +1210,7 @@
         <v>-1</v>
       </c>
       <c r="D47">
-        <v>0.852</v>
+        <v>0.853</v>
       </c>
       <c r="E47">
         <v>0.988</v>
@@ -1228,7 +1228,7 @@
         <v>-1</v>
       </c>
       <c r="D48">
-        <v>0.854</v>
+        <v>0.855</v>
       </c>
       <c r="E48">
         <v>0.988</v>
@@ -1264,7 +1264,7 @@
         <v>-1</v>
       </c>
       <c r="D50">
-        <v>0.866</v>
+        <v>0.864</v>
       </c>
       <c r="E50">
         <v>0.988</v>
@@ -1282,7 +1282,7 @@
         <v>-1</v>
       </c>
       <c r="D51">
-        <v>0.867</v>
+        <v>0.866</v>
       </c>
       <c r="E51">
         <v>0.988</v>
@@ -1290,17 +1290,17 @@
     </row>
     <row r="52">
       <c r="A52" s="2">
-        <f>HYPERLINK("pathways/Porphyrin_Metabolism.csv","Porphyrin Metabolism")</f>
+        <f>HYPERLINK("pathways/Mitochondrial_Electron_Transport_Chain.csv","Mitochondrial Electron Transport Chain")</f>
         <v>0</v>
       </c>
       <c r="B52">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C52">
         <v>-1</v>
       </c>
       <c r="D52">
-        <v>0.889</v>
+        <v>0.887</v>
       </c>
       <c r="E52">
         <v>0.988</v>
@@ -1308,17 +1308,17 @@
     </row>
     <row r="53">
       <c r="A53" s="2">
-        <f>HYPERLINK("pathways/Mitochondrial_Electron_Transport_Chain.csv","Mitochondrial Electron Transport Chain")</f>
+        <f>HYPERLINK("pathways/Porphyrin_Metabolism.csv","Porphyrin Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B53">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C53">
         <v>-1</v>
       </c>
       <c r="D53">
-        <v>0.889</v>
+        <v>0.888</v>
       </c>
       <c r="E53">
         <v>0.988</v>
@@ -1336,7 +1336,7 @@
         <v>-1</v>
       </c>
       <c r="D54">
-        <v>0.9</v>
+        <v>0.899</v>
       </c>
       <c r="E54">
         <v>0.988</v>
@@ -1344,17 +1344,17 @@
     </row>
     <row r="55">
       <c r="A55" s="2">
-        <f>HYPERLINK("pathways/Thyroid_hormone_synthesis.csv","Thyroid hormone synthesis")</f>
+        <f>HYPERLINK("pathways/Glutamate_Metabolism.csv","Glutamate Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B55">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C55">
         <v>-1</v>
       </c>
       <c r="D55">
-        <v>0.901</v>
+        <v>0.9</v>
       </c>
       <c r="E55">
         <v>0.988</v>
@@ -1362,17 +1362,17 @@
     </row>
     <row r="56">
       <c r="A56" s="2">
-        <f>HYPERLINK("pathways/Alanine_Metabolism.csv","Alanine Metabolism")</f>
+        <f>HYPERLINK("pathways/Thyroid_hormone_synthesis.csv","Thyroid hormone synthesis")</f>
         <v>0</v>
       </c>
       <c r="B56">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C56">
         <v>-1</v>
       </c>
       <c r="D56">
-        <v>0.902</v>
+        <v>0.901</v>
       </c>
       <c r="E56">
         <v>0.988</v>
@@ -1380,17 +1380,17 @@
     </row>
     <row r="57">
       <c r="A57" s="2">
-        <f>HYPERLINK("pathways/Lysine_Degradation.csv","Lysine Degradation")</f>
+        <f>HYPERLINK("pathways/Alanine_Metabolism.csv","Alanine Metabolism")</f>
         <v>0</v>
       </c>
       <c r="B57">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C57">
         <v>-1</v>
       </c>
       <c r="D57">
-        <v>0.902</v>
+        <v>0.901</v>
       </c>
       <c r="E57">
         <v>0.988</v>
@@ -1398,11 +1398,11 @@
     </row>
     <row r="58">
       <c r="A58" s="2">
-        <f>HYPERLINK("pathways/Glutamate_Metabolism.csv","Glutamate Metabolism")</f>
+        <f>HYPERLINK("pathways/Lysine_Degradation.csv","Lysine Degradation")</f>
         <v>0</v>
       </c>
       <c r="B58">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C58">
         <v>-1</v>
@@ -1426,7 +1426,7 @@
         <v>-1</v>
       </c>
       <c r="D59">
-        <v>0.905</v>
+        <v>0.904</v>
       </c>
       <c r="E59">
         <v>0.988</v>
@@ -1444,7 +1444,7 @@
         <v>-1</v>
       </c>
       <c r="D60">
-        <v>0.91</v>
+        <v>0.909</v>
       </c>
       <c r="E60">
         <v>0.988</v>
@@ -1462,7 +1462,7 @@
         <v>-1</v>
       </c>
       <c r="D61">
-        <v>0.915</v>
+        <v>0.914</v>
       </c>
       <c r="E61">
         <v>0.988</v>
@@ -1480,7 +1480,7 @@
         <v>-1</v>
       </c>
       <c r="D62">
-        <v>0.915</v>
+        <v>0.914</v>
       </c>
       <c r="E62">
         <v>0.988</v>
@@ -1498,7 +1498,7 @@
         <v>-1</v>
       </c>
       <c r="D63">
-        <v>0.915</v>
+        <v>0.914</v>
       </c>
       <c r="E63">
         <v>0.988</v>
@@ -1516,7 +1516,7 @@
         <v>-1</v>
       </c>
       <c r="D64">
-        <v>0.92</v>
+        <v>0.919</v>
       </c>
       <c r="E64">
         <v>0.988</v>
@@ -1552,7 +1552,7 @@
         <v>-1</v>
       </c>
       <c r="D66">
-        <v>0.942</v>
+        <v>0.941</v>
       </c>
       <c r="E66">
         <v>0.988</v>

</xml_diff>